<commit_message>
DataLoadManager 삭제, 여러 기존 Data 클래스 삭제
</commit_message>
<xml_diff>
--- a/Assets/100_Data/XlsxFiles/Ground_Data.xlsx
+++ b/Assets/100_Data/XlsxFiles/Ground_Data.xlsx
@@ -19,30 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>HP</t>
   </si>
   <si>
-    <t>stone</t>
-  </si>
-  <si>
     <t>Light_Brown[Light_Brown]</t>
   </si>
   <si>
-    <t>stone;iron</t>
-  </si>
-  <si>
     <t>Deep_Brown[Deep_Brown]</t>
   </si>
   <si>
-    <t>stone;iron;gold</t>
-  </si>
-  <si>
     <t>Lava_Earth[Lava_Earth]</t>
-  </si>
-  <si>
-    <t>diamond</t>
   </si>
   <si>
     <t>Id</t>
@@ -79,6 +67,14 @@
   </si>
   <si>
     <t>SpriteAddressable</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001;1003</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001;1003;1005</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1016,7 +1012,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1024,30 +1020,32 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="33.25" customWidth="1"/>
+    <col min="7" max="7" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1055,7 +1053,7 @@
         <v>5001</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1066,11 +1064,11 @@
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>1001</v>
+      </c>
+      <c r="G2" t="s">
         <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1078,7 +1076,7 @@
         <v>5002</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -1090,10 +1088,10 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1101,7 +1099,7 @@
         <v>5003</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>11</v>
@@ -1113,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1124,7 +1122,7 @@
         <v>5004</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1135,11 +1133,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>7</v>
+      <c r="F5">
+        <v>1007</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>